<commit_message>
add get api method: get conversation by id, get profile by userid, get groups conversation, get friend requests, get friends, get blocked users
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE4B925-53AC-4857-8575-F1C2E19D0FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E08B0EC-3C7F-4936-958F-19CF37DB32FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="122">
   <si>
     <t>POST</t>
   </si>
@@ -47,9 +47,6 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>DELETE</t>
-  </si>
-  <si>
     <t>/api/auth</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>/friends</t>
   </si>
   <si>
-    <t>/friends/:phone</t>
-  </si>
-  <si>
     <t>/block/:userId</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Lấy danh sách bạn</t>
   </si>
   <si>
-    <t>Lấy thông tin chi tiết bạn bằng phone</t>
-  </si>
-  <si>
     <t>Block bằng userId</t>
   </si>
   <si>
@@ -390,6 +381,27 @@
   </si>
   <si>
     <t>Tạo bình chọn?</t>
+  </si>
+  <si>
+    <t>/get-profile/:userId</t>
+  </si>
+  <si>
+    <t>:userId = userId (bên được xem)</t>
+  </si>
+  <si>
+    <t>Chưa test</t>
+  </si>
+  <si>
+    <t>Lấy profile (khác get) bằng userId</t>
+  </si>
+  <si>
+    <t>/forget-password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quên mật khẩu </t>
+  </si>
+  <si>
+    <t>{ phone, newPassword }</t>
   </si>
 </sst>
 </file>
@@ -805,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -824,33 +836,33 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -858,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -875,19 +887,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -895,16 +907,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -912,90 +924,88 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1003,62 +1013,62 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1066,19 +1076,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1086,170 +1096,179 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1257,67 +1276,70 @@
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>63</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="8" t="s">
+      <c r="G29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1325,96 +1347,99 @@
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1422,39 +1447,39 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1462,90 +1487,90 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="6" t="s">
+      <c r="G41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1553,39 +1578,39 @@
         <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1593,19 +1618,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1613,19 +1638,19 @@
         <v>2</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F46" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1633,19 +1658,19 @@
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1653,49 +1678,69 @@
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51">
+      <c r="B50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
         <f>COUNTIF(F:F,"x")</f>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD50 A51:A52 C51:XFD52 A53:XFD1048576">
+  <conditionalFormatting sqref="A52:A53 C52:XFD53 A54:XFD1048576 A1:XFD51">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>
@@ -1703,14 +1748,15 @@
       <formula>$F1="o"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
+  <conditionalFormatting sqref="B52">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$F52="x"</formula>
+      <formula>$F53="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>$F52="o"</formula>
+      <formula>$F53="o"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add api group-related and friend request-related
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E08B0EC-3C7F-4936-958F-19CF37DB32FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B8090E-CCA2-4BE5-B300-6E2743C3CB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="136">
   <si>
     <t>POST</t>
   </si>
@@ -395,13 +395,55 @@
     <t>Lấy profile (khác get) bằng userId</t>
   </si>
   <si>
-    <t>/forget-password</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quên mật khẩu </t>
   </si>
   <si>
     <t>{ phone, newPassword }</t>
+  </si>
+  <si>
+    <t>/check-used-phone/:phone</t>
+  </si>
+  <si>
+    <t>Kiểm tra phone đã dùng chưa</t>
+  </si>
+  <si>
+    <t>/forgot-password</t>
+  </si>
+  <si>
+    <t>ai cũng được thêm</t>
+  </si>
+  <si>
+    <t>Chỉ trưởng nhóm và phó nhóm mới được xóa</t>
+  </si>
+  <si>
+    <t>chỉ trưởng nhóm mới được</t>
+  </si>
+  <si>
+    <t>nếu trưởng nhóm out thì phải chọn 1 người chuyển trưởng nhóm</t>
+  </si>
+  <si>
+    <t>/group/:conversationId/set-co-owner</t>
+  </si>
+  <si>
+    <t>{coOwnerIds:["userId1","userId2"]}</t>
+  </si>
+  <si>
+    <t>Set những ai làm phó nhóm</t>
+  </si>
+  <si>
+    <t>/group/:conversationId/set-owner/:userId</t>
+  </si>
+  <si>
+    <t>Set ai làm trưởng nhóm</t>
+  </si>
+  <si>
+    <t>:userId= userId</t>
+  </si>
+  <si>
+    <t>Cắt chức phó nhóm</t>
+  </si>
+  <si>
+    <t>/group/:conversationId/remove-co-owner/:userId</t>
   </si>
 </sst>
 </file>
@@ -817,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -947,16 +989,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H7" s="9"/>
     </row>
@@ -1052,7 +1094,7 @@
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1073,22 +1115,19 @@
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>122</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1096,16 +1135,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>108</v>
@@ -1116,39 +1155,39 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1156,13 +1195,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>30</v>
@@ -1174,24 +1210,27 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1199,73 +1238,76 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>58</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="9" t="s">
+      <c r="F23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>108</v>
@@ -1273,19 +1315,16 @@
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>108</v>
@@ -1296,87 +1335,87 @@
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>60</v>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1384,13 +1423,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>30</v>
@@ -1402,18 +1438,18 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>30</v>
@@ -1421,19 +1457,22 @@
       <c r="G33" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H33" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>30</v>
@@ -1444,19 +1483,19 @@
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>108</v>
@@ -1467,39 +1506,45 @@
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>80</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1507,61 +1552,91 @@
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>19</v>
+      <c r="F41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>79</v>
@@ -1572,82 +1647,56 @@
       <c r="G42" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>108</v>
+      <c r="H42" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>108</v>
@@ -1655,19 +1704,19 @@
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>108</v>
@@ -1675,16 +1724,16 @@
     </row>
     <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
@@ -1698,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>15</v>
@@ -1715,13 +1764,16 @@
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>114</v>
+        <v>96</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>15</v>
@@ -1730,17 +1782,94 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>104</v>
       </c>
-      <c r="C52">
+      <c r="C56">
         <f>COUNTIF(F:F,"x")</f>
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A52:A53 C52:XFD53 A54:XFD1048576 A1:XFD51">
+  <conditionalFormatting sqref="A56:A57 C56:XFD57 A58:XFD1048576 A1:XFD38 A41:XFD55 A39:C40 E39:XFD40">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>
@@ -1748,12 +1877,12 @@
       <formula>$F1="o"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
+  <conditionalFormatting sqref="B56 D39:D40">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$F53="x"</formula>
+      <formula>$F40="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>$F53="o"</formula>
+      <formula>$F40="o"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update api-guide, fix bug api cant change group name
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377E33F7-DBF4-4404-99CD-369BFFC8EBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D3E13C-4C13-40A5-9247-B8F21C231D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="1065" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="825" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2111,7 +2111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2139,6 +2139,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2458,27 +2459,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D41" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.125" customWidth="1"/>
     <col min="5" max="5" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.125" style="12" customWidth="1"/>
     <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="148.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2517,14 +2518,14 @@
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2537,14 +2538,14 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2555,7 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -2564,7 +2565,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2577,7 +2578,7 @@
       <c r="E6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -2587,7 +2588,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2600,14 +2601,14 @@
       <c r="E7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
@@ -2617,7 +2618,7 @@
       <c r="C8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -2627,7 +2628,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -2643,14 +2644,14 @@
       <c r="E9" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -2663,14 +2664,14 @@
       <c r="E10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -2680,14 +2681,14 @@
       <c r="C11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -2697,14 +2698,14 @@
       <c r="C12" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -2714,14 +2715,14 @@
       <c r="C13" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -2731,11 +2732,11 @@
       <c r="C14" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -2748,11 +2749,11 @@
       <c r="E15" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2765,19 +2766,20 @@
       <c r="E16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17"/>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -2803,7 +2805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -2816,14 +2818,14 @@
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
@@ -2836,14 +2838,14 @@
       <c r="D21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -2856,7 +2858,7 @@
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -2866,7 +2868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -2879,14 +2881,14 @@
       <c r="E23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -2899,7 +2901,7 @@
       <c r="E24" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2909,7 +2911,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -2922,14 +2924,14 @@
       <c r="E25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
@@ -2939,7 +2941,7 @@
       <c r="C26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -2949,7 +2951,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -2962,7 +2964,7 @@
       <c r="D27" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -2972,7 +2974,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2985,7 +2987,7 @@
       <c r="D28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -2995,7 +2997,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
@@ -3008,7 +3010,7 @@
       <c r="D29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -3018,7 +3020,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
@@ -3028,7 +3030,7 @@
       <c r="C30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -3038,7 +3040,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -3051,7 +3053,7 @@
       <c r="D31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -3061,7 +3063,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -3071,7 +3073,7 @@
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -3081,7 +3083,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -3094,7 +3096,7 @@
       <c r="D33" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -3104,7 +3106,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -3117,7 +3119,7 @@
       <c r="D34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -3127,12 +3129,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>40</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>1</v>
       </c>
@@ -3168,14 +3170,14 @@
       <c r="C38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
@@ -3185,7 +3187,7 @@
       <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -3195,7 +3197,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>1</v>
       </c>
@@ -3208,7 +3210,7 @@
       <c r="D40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -3218,7 +3220,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
@@ -3231,14 +3233,14 @@
       <c r="E41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" s="2" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -3251,14 +3253,14 @@
       <c r="E42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -3271,7 +3273,7 @@
       <c r="D43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -3281,7 +3283,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
@@ -3294,7 +3296,7 @@
       <c r="D44" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G44" s="2" t="s">
@@ -3304,7 +3306,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -3318,14 +3320,14 @@
       <c r="E45" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
@@ -3338,11 +3340,11 @@
       <c r="D46" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F46" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
@@ -3355,14 +3357,14 @@
       <c r="D47" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -3375,7 +3377,7 @@
       <c r="D48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -3385,7 +3387,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
@@ -3398,7 +3400,7 @@
       <c r="D49" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -3408,7 +3410,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>2</v>
       </c>
@@ -3424,11 +3426,11 @@
       <c r="E50" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F50" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -3444,14 +3446,14 @@
       <c r="E51" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -3467,19 +3469,20 @@
       <c r="E52" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>40</v>
       </c>
@@ -3505,7 +3508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>1</v>
       </c>
@@ -3518,14 +3521,14 @@
       <c r="D56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -3538,14 +3541,14 @@
       <c r="E57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
@@ -3558,14 +3561,14 @@
       <c r="E58" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -3578,14 +3581,14 @@
       <c r="D59" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -3598,14 +3601,14 @@
       <c r="D60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -3618,14 +3621,14 @@
       <c r="D61" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -3638,14 +3641,14 @@
       <c r="D62" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -3658,14 +3661,14 @@
       <c r="D63" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -3675,19 +3678,20 @@
       <c r="C64" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>40</v>
       </c>
@@ -3713,7 +3717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>1</v>
       </c>
@@ -3726,7 +3730,7 @@
       <c r="D69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G69" s="2" t="s">
@@ -3736,13 +3740,13 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="H70" s="13" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>100</v>
       </c>
@@ -3754,74 +3758,74 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H72" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H73" s="13" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H74" s="14"/>
     </row>
-    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H75" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H76" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H77" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H78" s="14"/>
     </row>
-    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H79" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H80" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="81" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H81" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H82" s="13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="83" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H83" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="84" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H84" s="13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="8:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H85" s="13" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A46:C47 E46:XFD47 A48:XFD69 A70:G70 I70:XFD85 A71:A72 C71:G72 A73:G85 A86:XFD1048576 A1:XFD45">
+  <conditionalFormatting sqref="A1:XFD45 A46:C47 E46:XFD47 A48:XFD69 A70:G70 I70:XFD85 A71:A72 C71:G72 A73:G85 A86:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
adjust api change avatar
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C94A8C-06CC-4F6C-975C-1C19384C7CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8CBAC-847E-4549-83F8-B5D4935A0CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>avatar</t>
+      <t>groupBackground</t>
     </r>
     <r>
       <rPr>
@@ -513,7 +513,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>', imageFile); cái này có trả về nguyên cái user luôn để cập nhật vào localstorage</t>
+      <t xml:space="preserve">', imageFile); </t>
     </r>
   </si>
   <si>
@@ -532,7 +532,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>groupBackground</t>
+      <t>groupAvatar</t>
     </r>
     <r>
       <rPr>
@@ -546,14 +546,1245 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>const formData = new FormData(); formData.append('</t>
+    <t>/api/notifcations</t>
+  </si>
+  <si>
+    <t>/conversation/:conversationId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy ra các notify của conversation </t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF80BBFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>messages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF80BBFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>notifications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD5D8E0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>await</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF81CFE0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>Promise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>([</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>fetch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF82D99F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>`/api/messages/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF2858C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>conversationId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF2858C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF82D99F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>()),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>fetch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF82D99F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>`/api/notifications/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF2858C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>conversationId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF2858C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF82D99F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>())</t>
+    </r>
+  </si>
+  <si>
+    <t>    ]);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF80BBFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>allContent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD5D8E0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD5D8E0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>messages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD5D8E0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>notifications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>].</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE0E3EE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>createdAt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD5D8E0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE0E3EE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>createdAt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>    );</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>allContent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>forEach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE0E3EE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>isNotification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>renderNotification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB38CFF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF29D79"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>renderMessage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDED47E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="163"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <t>    });</t>
+  </si>
+  <si>
+    <t>Bên FE vừa lấy message vừa lấy notify nhe, xong merge lại rồi render lên, code mẫu nè</t>
+  </si>
+  <si>
+    <t>AT chỉ có 1h nhma RT là 7 ngày nhe</t>
+  </si>
+  <si>
+    <t>Mỗi cái otp chỉ được thử 3 lần, quá 3 lần thì phải yêu cầu otp mới nhe, chỉ được verify tối đa 5 lần mỗi 15 phút, do lưu trong Ram của server nên restart là đc thử tiếp nhe</t>
+  </si>
+  <si>
+    <t>Tạo cái blacklistkey bằng jit xong nhét vô cache có hạn 24h, sau này nếu mw auth mà có đứa xài có jit nằm trong cái cache này thì bị chặn</t>
+  </si>
+  <si>
+    <t>QR có hạn 5p thôi, 5p rồi thì QR hết hạn, quét trước đó rồi mà để tới giờ mới verify confirm thì cũng ko đc. Nên làm thêm cái gì đó để refresh QR</t>
+  </si>
+  <si>
+    <t>Đổi trong phiên đăng nhập, đổi xong refresh lại token</t>
+  </si>
+  <si>
+    <t>cũng như cái logout, nhét jit cũ vô blacklist rồi tạo mới cặp jwt</t>
+  </si>
+  <si>
+    <t>Lấy profile (khác get user) bằng userId</t>
+  </si>
+  <si>
+    <t>/send-otp-forgot-password</t>
+  </si>
+  <si>
+    <t>/verify-otp-forgot-password</t>
+  </si>
+  <si>
+    <t>Gửi otp để chạy tiếp chức năng quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Xác thực otp quên mật khẩu</t>
+  </si>
+  <si>
+    <t>{phone}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/generate-qr-token  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trả về res qr token để tạo qr đăng nhập </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <i/>
-        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
@@ -561,7 +1792,21 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>groupAvatar</t>
+      <t>(bên đăng nhập)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bên quét</t>
     </r>
     <r>
       <rPr>
@@ -571,1246 +1816,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">', imageFile); </t>
-    </r>
-  </si>
-  <si>
-    <t>/api/notifcations</t>
-  </si>
-  <si>
-    <t>/conversation/:conversationId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lấy ra các notify của conversation </t>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>const</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> [</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF80BBFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>messages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF80BBFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>notifications</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD5D8E0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>await</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF81CFE0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>Promise</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>([</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>fetch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF82D99F"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>`/api/messages/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF2858C"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>conversationId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF2858C"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF82D99F"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>`</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>json</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>()),</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>fetch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF82D99F"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>`/api/notifications/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF2858C"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>conversationId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF2858C"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF82D99F"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>`</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>json</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>())</t>
-    </r>
-  </si>
-  <si>
-    <t>    ]);</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>const</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF80BBFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>allContent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD5D8E0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> [</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD5D8E0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>messages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD5D8E0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>notifications</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>].</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>sort</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>((</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>new</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFE0E3EE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>createdAt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD5D8E0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>new</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFE0E3EE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>createdAt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>    );</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>allContent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>forEach</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>if</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFE0E3EE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>isNotification</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>) {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>renderNotification</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        } </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB38CFF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>else</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF29D79"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>renderMessage</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDED47E"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>item</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="163"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <t>        }</t>
-  </si>
-  <si>
-    <t>    });</t>
-  </si>
-  <si>
-    <t>Bên FE vừa lấy message vừa lấy notify nhe, xong merge lại rồi render lên, code mẫu nè</t>
-  </si>
-  <si>
-    <t>AT chỉ có 1h nhma RT là 7 ngày nhe</t>
-  </si>
-  <si>
-    <t>Mỗi cái otp chỉ được thử 3 lần, quá 3 lần thì phải yêu cầu otp mới nhe, chỉ được verify tối đa 5 lần mỗi 15 phút, do lưu trong Ram của server nên restart là đc thử tiếp nhe</t>
-  </si>
-  <si>
-    <t>Tạo cái blacklistkey bằng jit xong nhét vô cache có hạn 24h, sau này nếu mw auth mà có đứa xài có jit nằm trong cái cache này thì bị chặn</t>
-  </si>
-  <si>
-    <t>QR có hạn 5p thôi, 5p rồi thì QR hết hạn, quét trước đó rồi mà để tới giờ mới verify confirm thì cũng ko đc. Nên làm thêm cái gì đó để refresh QR</t>
-  </si>
-  <si>
-    <t>Đổi trong phiên đăng nhập, đổi xong refresh lại token</t>
-  </si>
-  <si>
-    <t>cũng như cái logout, nhét jit cũ vô blacklist rồi tạo mới cặp jwt</t>
-  </si>
-  <si>
-    <t>Lấy profile (khác get user) bằng userId</t>
-  </si>
-  <si>
-    <t>/send-otp-forgot-password</t>
-  </si>
-  <si>
-    <t>/verify-otp-forgot-password</t>
-  </si>
-  <si>
-    <t>Gửi otp để chạy tiếp chức năng quên mật khẩu</t>
-  </si>
-  <si>
-    <t>Xác thực otp quên mật khẩu</t>
-  </si>
-  <si>
-    <t>{phone}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/generate-qr-token  </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trả về res qr token để tạo qr đăng nhập </t>
-    </r>
+      <t xml:space="preserve"> qr để xác thực (nhét userId vào cache)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1821,21 +1830,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(bên đăng nhập)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bên quét</t>
+      <t xml:space="preserve">Bên quét </t>
     </r>
     <r>
       <rPr>
@@ -1845,7 +1840,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> qr để xác thực (nhét userId vào cache)</t>
+      <t>xác nhận đăng nhập (confirm lần nữa)</t>
     </r>
   </si>
   <si>
@@ -1859,7 +1854,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Bên quét </t>
+      <t>Bên đăng nhập</t>
     </r>
     <r>
       <rPr>
@@ -1869,8 +1864,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>xác nhận đăng nhập (confirm lần nữa)</t>
-    </r>
+      <t xml:space="preserve"> xác nhận trạng thái qr để đăng nhập</t>
+    </r>
+  </si>
+  <si>
+    <t>Update avt trên điện thoại</t>
+  </si>
+  <si>
+    <t>Update infor trên điện thoại</t>
+  </si>
+  <si>
+    <t>{isMale, birhtday, fullname, imageBase64}</t>
+  </si>
+  <si>
+    <t>{isMale, birhtday, fullname}</t>
+  </si>
+  <si>
+    <t>imageBase64</t>
   </si>
   <si>
     <r>
@@ -1883,7 +1893,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Bên đăng nhập</t>
+      <t>/mobile</t>
     </r>
     <r>
       <rPr>
@@ -1893,23 +1903,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> xác nhận trạng thái qr để đăng nhập</t>
-    </r>
-  </si>
-  <si>
-    <t>Update avt trên điện thoại</t>
-  </si>
-  <si>
-    <t>Update infor trên điện thoại</t>
-  </si>
-  <si>
-    <t>{isMale, birhtday, fullname, imageBase64}</t>
-  </si>
-  <si>
-    <t>{isMale, birhtday, fullname}</t>
-  </si>
-  <si>
-    <t>imageBase64</t>
+      <t>/update-user/info</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1932,13 +1927,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/update-user/info</t>
-    </r>
-  </si>
-  <si>
+      <t>/update-user/avatar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>const formData = new FormData(); formData.append('</t>
+    </r>
     <r>
       <rPr>
         <b/>
+        <i/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
@@ -1946,7 +1946,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/mobile</t>
+      <t>avatar</t>
     </r>
     <r>
       <rPr>
@@ -1956,7 +1956,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/update-user/avatar</t>
+      <t>', imageFile); await fetch('/api/users/update-user/avatar', { method: 'PUT',headers: {   'Authorization': `Bearer ${token}`}, body: formData}); cái này có trả về nguyên cái user luôn để cập nhật vào localstorage</t>
     </r>
   </si>
 </sst>
@@ -2528,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,7 +2540,7 @@
     <col min="5" max="5" width="57.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.125" style="12" customWidth="1"/>
     <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="148.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="222.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>103</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>103</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2745,16 +2745,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>135</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>27</v>
@@ -2782,7 +2782,7 @@
         <v>136</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>27</v>
@@ -2799,7 +2799,7 @@
         <v>137</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>27</v>
@@ -2810,13 +2810,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>27</v>
@@ -2827,10 +2827,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>133</v>
@@ -2977,7 +2977,7 @@
         <v>103</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>43</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>27</v>
@@ -3005,13 +3005,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>27</v>
@@ -3025,13 +3025,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>27</v>
@@ -3068,7 +3068,7 @@
         <v>110</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>111</v>
@@ -3559,7 +3559,7 @@
         <v>27</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3582,7 +3582,7 @@
         <v>27</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
     </row>
     <row r="69" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F69" s="16"/>
     </row>
@@ -3831,10 +3831,10 @@
         <v>1</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>74</v>
@@ -3846,13 +3846,13 @@
         <v>103</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="H72" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3864,17 +3864,17 @@
         <v>7</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H74" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H75" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3882,17 +3882,17 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H77" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H78" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H79" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3900,41 +3900,41 @@
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H81" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H82" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H83" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H84" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H85" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H86" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H87" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A48:C49 E48:XFD49 A50:XFD71 A72:G72 I72:XFD87 A73:A74 C73:G74 A75:G87 A88:XFD1048576 A1:XFD47">
+  <conditionalFormatting sqref="A1:XFD47 A48:C49 E48:XFD49 A50:XFD71 A72:G72 I72:XFD87 A73:A74 C73:G74 A75:G87 A88:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
modify model using date change to isodate, adjust get messages from conversation logic
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78633080-8126-4B5E-8A86-421225CFA819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DFBF14-ADBA-49F9-8A64-53F3E885E5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="825" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="196">
   <si>
     <t>POST</t>
   </si>
@@ -1959,18 +1959,29 @@
       </rPr>
       <t>/update-info</t>
     </r>
+  </si>
+  <si>
+    <t>cái này trả thêm 2 cái là hasMore (true, false) và nextCursor là timestamp tin nhắn cũ nhất của lần gọi này (limit 20), khi request thì thêm query lastMesssageTime vào cái api (không có thì mặc định lấy 20 cái mới nhất)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2182,34 +2193,34 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2529,8 +2540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,6 +3647,9 @@
       </c>
       <c r="G58" s="2" t="s">
         <v>103</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adjust api block/unblock, update api guide
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DFBF14-ADBA-49F9-8A64-53F3E885E5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D600667-8C9C-4FF5-8240-E2F2D41B630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="825" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="203">
   <si>
     <t>POST</t>
   </si>
@@ -149,9 +149,6 @@
     <t>/friend-requests/send-request/:userId</t>
   </si>
   <si>
-    <t>/friend-requests</t>
-  </si>
-  <si>
     <t>/friend-requests/accept-request/:requestId</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>Gửi request kết bạn</t>
-  </si>
-  <si>
-    <t>Lấy danh sách request</t>
   </si>
   <si>
     <t>Chấp nhận request</t>
@@ -1962,6 +1956,33 @@
   </si>
   <si>
     <t>cái này trả thêm 2 cái là hasMore (true, false) và nextCursor là timestamp tin nhắn cũ nhất của lần gọi này (limit 20), khi request thì thêm query lastMesssageTime vào cái api (không có thì mặc định lấy 20 cái mới nhất)</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/friend-requests-sent</t>
+  </si>
+  <si>
+    <t>/friend-requests-received</t>
+  </si>
+  <si>
+    <t>Lấy danh sách request đã nhận</t>
+  </si>
+  <si>
+    <t>Lấy danh sách request đã gửi</t>
+  </si>
+  <si>
+    <t>/friend-requests/retrieve-request/:userId</t>
+  </si>
+  <si>
+    <t>Thu hồi request</t>
+  </si>
+  <si>
+    <t>:userId = userId (bên bị block)</t>
   </si>
 </sst>
 </file>
@@ -2538,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,7 +2583,7 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -2603,7 +2624,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2623,7 +2644,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2640,10 +2661,10 @@
         <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2651,22 +2672,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2674,39 +2695,39 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2714,22 +2735,22 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2737,19 +2758,19 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2757,16 +2778,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2774,16 +2795,16 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2791,16 +2812,16 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2808,10 +2829,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>27</v>
@@ -2822,13 +2843,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>179</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>27</v>
@@ -2839,13 +2860,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>180</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>27</v>
@@ -2862,7 +2883,7 @@
     </row>
     <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
@@ -2891,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -2903,7 +2924,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2911,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -2923,7 +2944,7 @@
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2931,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>25</v>
@@ -2943,7 +2964,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>28</v>
@@ -2957,16 +2978,16 @@
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2977,19 +2998,19 @@
         <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3000,16 +3021,16 @@
         <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3017,19 +3038,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3037,19 +3058,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3060,16 +3081,16 @@
         <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3077,22 +3098,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3103,19 +3124,19 @@
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>202</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3126,19 +3147,19 @@
         <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>54</v>
+        <v>202</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3149,16 +3170,16 @@
         <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3169,19 +3190,22 @@
         <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3189,133 +3213,135 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>112</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>53</v>
+        <v>198</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H41" s="8" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3323,146 +3349,145 @@
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="B46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="F46" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="2" t="s">
-        <v>122</v>
+        <v>68</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3470,19 +3495,20 @@
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3490,22 +3516,16 @@
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>74</v>
+        <v>125</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3513,22 +3533,19 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>74</v>
+        <v>123</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3536,19 +3553,22 @@
         <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3556,22 +3576,22 @@
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>148</v>
+        <v>72</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="G53" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="H53" s="2" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3579,157 +3599,160 @@
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F54" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B57" s="6" t="s">
+    </row>
+    <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E59" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F59" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G59" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H59" s="6" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3737,19 +3760,19 @@
         <v>2</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3757,19 +3780,19 @@
         <v>2</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3777,179 +3800,219 @@
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>109</v>
+        <v>91</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="D73" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="12"/>
+      <c r="H74" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="H72" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C73">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75">
         <f>COUNTIF(F:F,"x")</f>
         <v>7</v>
       </c>
-      <c r="H73" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H74" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H75" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H76" s="14"/>
+      <c r="H76" s="13" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H77" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H78" s="13" t="s">
-        <v>160</v>
-      </c>
+      <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H79" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H80" s="14"/>
+      <c r="H80" s="13" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H81" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H82" s="13" t="s">
-        <v>163</v>
-      </c>
+      <c r="H82" s="14"/>
     </row>
     <row r="83" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H83" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H84" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H85" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H86" s="13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H87" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="13" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD47 A48:C49 E48:XFD49 A50:XFD71 A72:G72 I72:XFD87 A73:A74 C73:G74 A75:G87 A88:XFD1048576">
+  <conditionalFormatting sqref="A50:C51 E50:XFD51 A52:XFD73 A74:G74 I74:XFD89 A75:A76 C75:G76 A77:G89 A90:XFD1048576 A1:XFD49">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>
@@ -3957,12 +4020,12 @@
       <formula>$F1="o"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D49 B73">
+  <conditionalFormatting sqref="D50:D51 B75">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$F49="x"</formula>
+      <formula>$F51="x"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>$F49="o"</formula>
+      <formula>$F51="o"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjust api get notification
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D600667-8C9C-4FF5-8240-E2F2D41B630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7C555-0157-4244-A0CA-8186272375B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="825" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="204">
   <si>
     <t>POST</t>
   </si>
@@ -1731,9 +1731,6 @@
     <t>    });</t>
   </si>
   <si>
-    <t>Bên FE vừa lấy message vừa lấy notify nhe, xong merge lại rồi render lên, code mẫu nè</t>
-  </si>
-  <si>
     <t>AT chỉ có 1h nhma RT là 7 ngày nhe</t>
   </si>
   <si>
@@ -1983,6 +1980,12 @@
   </si>
   <si>
     <t>:userId = userId (bên bị block)</t>
+  </si>
+  <si>
+    <t>{ oldestTime, newestTime } (query ko phải body)</t>
+  </si>
+  <si>
+    <t>Bên FE vừa lấy message vừa lấy notify nhe, xong merge lại rồi render lên, code mẫu nè, truyền vào thêm newest Time và oldestTime (2 cái này option), truyền oldest để lấy mấy message mới hơn, giới lại bởi newest</t>
   </si>
 </sst>
 </file>
@@ -2561,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="H64" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2627,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2664,7 +2667,7 @@
         <v>101</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2687,7 +2690,7 @@
         <v>101</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2727,7 +2730,7 @@
         <v>102</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2770,7 +2773,7 @@
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2778,16 +2781,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2798,7 +2801,7 @@
         <v>133</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>27</v>
@@ -2815,7 +2818,7 @@
         <v>134</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>27</v>
@@ -2832,7 +2835,7 @@
         <v>135</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>27</v>
@@ -2843,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>27</v>
@@ -2860,10 +2863,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>131</v>
@@ -3010,7 +3013,7 @@
         <v>101</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3024,7 +3027,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>27</v>
@@ -3038,13 +3041,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>27</v>
@@ -3058,13 +3061,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>27</v>
@@ -3101,7 +3104,7 @@
         <v>108</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>109</v>
@@ -3127,7 +3130,7 @@
         <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>27</v>
@@ -3150,7 +3153,7 @@
         <v>45</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>27</v>
@@ -3196,7 +3199,7 @@
         <v>52</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>27</v>
@@ -3213,10 +3216,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>27</v>
@@ -3231,10 +3234,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>27</v>
@@ -3248,13 +3251,13 @@
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>51</v>
@@ -3712,7 +3715,7 @@
         <v>101</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3917,6 +3920,9 @@
       <c r="D73" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="E73" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="F73" s="9" t="s">
         <v>27</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>101</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4012,7 +4018,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A50:C51 E50:XFD51 A52:XFD73 A74:G74 I74:XFD89 A75:A76 C75:G76 A77:G89 A90:XFD1048576 A1:XFD49">
+  <conditionalFormatting sqref="A1:XFD49 A50:C51 E50:XFD51 A52:XFD73 A74:G74 I74:XFD89 A75:A76 C75:G76 A77:G89 A90:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F1="x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update api end point send file, update api guide
</commit_message>
<xml_diff>
--- a/api-guide.xlsx
+++ b/api-guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sophy_Chatapp_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7C555-0157-4244-A0CA-8186272375B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144CDFB2-59B5-490D-BBBB-70C47B097BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="825" windowWidth="26325" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="209">
   <si>
     <t>POST</t>
   </si>
@@ -275,9 +275,6 @@
     <t>/send</t>
   </si>
   <si>
-    <t>/send-with-attachment</t>
-  </si>
-  <si>
     <t>/:messageId/recall</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>Gửi tin nhắn vào một conversation</t>
   </si>
   <si>
-    <t>Sử dụng gửi tin nhắn có đính kèm</t>
-  </si>
-  <si>
     <t>Thu hồi tin nhắn (không ai được xem)</t>
   </si>
   <si>
@@ -321,9 +315,6 @@
   </si>
   <si>
     <t>{conversationId, content}</t>
-  </si>
-  <si>
-    <t>{conversationId, content, attachments?}</t>
   </si>
   <si>
     <t>/send-poll?</t>
@@ -1986,6 +1977,30 @@
   </si>
   <si>
     <t>Bên FE vừa lấy message vừa lấy notify nhe, xong merge lại rồi render lên, code mẫu nè, truyền vào thêm newest Time và oldestTime (2 cái này option), truyền oldest để lấy mấy message mới hơn, giới lại bởi newest</t>
+  </si>
+  <si>
+    <t>/send-with-image</t>
+  </si>
+  <si>
+    <t>/send-image</t>
+  </si>
+  <si>
+    <t>/send-file</t>
+  </si>
+  <si>
+    <t>Gửi chỉ 1 hình ảnh, không có text (content =null)</t>
+  </si>
+  <si>
+    <t>Gửi chỉ 1 file/video, không có text</t>
+  </si>
+  <si>
+    <t>Sử dụng gửi tin nhắn có đính kèm 1 ảnh duy nhất</t>
+  </si>
+  <si>
+    <t>{conversationId, content} + formData</t>
+  </si>
+  <si>
+    <t>{conversationId} + formData</t>
   </si>
 </sst>
 </file>
@@ -2249,7 +2264,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2562,10 +2605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H64" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +2670,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2647,7 +2690,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2664,10 +2707,10 @@
         <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2675,22 +2718,22 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2698,39 +2741,39 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2738,22 +2781,22 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2761,19 +2804,19 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2781,16 +2824,16 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2798,16 +2841,16 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2815,16 +2858,16 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2832,10 +2875,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>27</v>
@@ -2846,13 +2889,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>27</v>
@@ -2863,13 +2906,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>27</v>
@@ -2915,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -2927,7 +2970,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2935,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -2947,7 +2990,7 @@
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2955,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>25</v>
@@ -2967,7 +3010,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>28</v>
@@ -2990,7 +3033,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3004,16 +3047,16 @@
         <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3027,13 +3070,13 @@
         <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3041,19 +3084,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3061,19 +3104,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3090,10 +3133,10 @@
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3101,22 +3144,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3130,16 +3173,16 @@
         <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3153,16 +3196,16 @@
         <v>45</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3179,10 +3222,10 @@
         <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3199,16 +3242,16 @@
         <v>52</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3216,16 +3259,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="F34" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H34" s="9"/>
     </row>
@@ -3234,30 +3277,30 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>51</v>
@@ -3266,7 +3309,7 @@
         <v>27</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H36" s="9"/>
     </row>
@@ -3287,10 +3330,10 @@
         <v>27</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3310,10 +3353,10 @@
         <v>27</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3361,7 +3404,7 @@
         <v>27</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3378,10 +3421,10 @@
         <v>27</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3401,10 +3444,10 @@
         <v>27</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3424,7 +3467,7 @@
         <v>27</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
@@ -3444,7 +3487,7 @@
         <v>27</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3464,10 +3507,10 @@
         <v>27</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3487,10 +3530,10 @@
         <v>27</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3498,20 +3541,20 @@
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3519,13 +3562,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>27</v>
@@ -3536,19 +3579,19 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3568,10 +3611,10 @@
         <v>27</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3591,10 +3634,10 @@
         <v>27</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3602,16 +3645,16 @@
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>27</v>
@@ -3622,22 +3665,22 @@
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="D55" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3645,22 +3688,22 @@
         <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3703,7 +3746,7 @@
         <v>77</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>72</v>
@@ -3712,10 +3755,10 @@
         <v>27</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3726,16 +3769,16 @@
         <v>78</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>27</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3743,59 +3786,59 @@
         <v>0</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>87</v>
+        <v>206</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>93</v>
+        <v>204</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>93</v>
+        <v>205</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3803,19 +3846,19 @@
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3823,19 +3866,19 @@
         <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="F66" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3843,195 +3886,251 @@
         <v>2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F68" s="9" t="s">
+      <c r="B70" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G68" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="G70" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73" s="16"/>
+    </row>
+    <row r="74" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="12"/>
+      <c r="H76" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="F71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F72" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="2" t="s">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77">
+        <f>COUNTIF(F:F,"x")</f>
+        <v>2</v>
+      </c>
+      <c r="H77" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="2" t="s">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H78" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
-      <c r="H74" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75">
-        <f>COUNTIF(F:F,"x")</f>
-        <v>7</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H76" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H77" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H79" s="13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H80" s="13" t="s">
-        <v>158</v>
-      </c>
+      <c r="H80" s="14"/>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H81" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H82" s="14"/>
+      <c r="H82" s="13" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="83" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H83" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H84" s="13" t="s">
-        <v>161</v>
-      </c>
+      <c r="H84" s="14"/>
     </row>
     <row r="85" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H85" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H86" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H87" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H88" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H89" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="13" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD49 A50:C51 E50:XFD51 A52:XFD73 A74:G74 I74:XFD89 A75:A76 C75:G76 A77:G89 A90:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A1:XFD49 A50:C51 E50:XFD51 A76:G76 I76:XFD91 A77:A78 C77:G78 A79:G91 A92:XFD1048576 A52:XFD62 A65:XFD75 A63:F64 H63:XFD64">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$F1="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$F1="o"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50:D51 B75">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="D50:D51 B77">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$F51="x"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$F51="o"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G64">
+    <cfRule type="expression" dxfId="3" priority="13">
+      <formula>$F63="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="14">
+      <formula>$F63="o"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G63">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$F63="x"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$F63="o"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>